<commit_message>
fixed errors and overview now working
</commit_message>
<xml_diff>
--- a/Snittbetyg - Beräkning.xlsx
+++ b/Snittbetyg - Beräkning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielamir/Desktop/StudyTimeAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6B6A12-2A19-7142-9FA2-24AFAEF580CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE254032-B496-5042-B26A-96BA696763F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>HP</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Fotonik</t>
   </si>
   <si>
-    <t>Programmering Fördjupningskurs</t>
-  </si>
-  <si>
     <t>Diskreta Strukturer i Datavetenskap</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Endimensionell Analys B2</t>
   </si>
   <si>
-    <t>Introduktion till artificiella neurala nätverk och deep learning</t>
-  </si>
-  <si>
     <t>Flerdimensionell Analys</t>
   </si>
   <si>
@@ -130,6 +124,24 @@
   </si>
   <si>
     <t>Betyg</t>
+  </si>
+  <si>
+    <t>Introduktion till artificiella neuronnätverk och deep learning</t>
+  </si>
+  <si>
+    <t>Programmeringsteknik Fördjupningskurs</t>
+  </si>
+  <si>
+    <t>Kandidatarbete</t>
+  </si>
+  <si>
+    <t>Programvaruutveckling i grupp</t>
+  </si>
+  <si>
+    <t>Datorer och Datoranvändning</t>
+  </si>
+  <si>
+    <t>Utvärdering av Programvarusystem</t>
   </si>
 </sst>
 </file>
@@ -165,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -294,11 +306,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -319,6 +353,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841D7259-A76A-2945-8CF6-F9C9DD122C8A}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -618,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -626,10 +662,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -640,10 +676,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -654,7 +690,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -668,7 +704,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -682,7 +718,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -696,10 +732,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -710,10 +746,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -724,10 +760,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -738,10 +774,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -752,10 +788,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -766,10 +802,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -780,10 +816,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
         <v>5</v>
@@ -794,10 +830,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -808,10 +844,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -822,10 +858,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -836,10 +872,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -850,10 +886,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -864,10 +900,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -878,10 +914,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -892,10 +928,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -906,10 +942,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -920,10 +956,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -934,16 +970,72 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
       </c>
       <c r="D24" s="1">
         <v>7.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D25" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D26" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D27" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>